<commit_message>
percentage sign added after each value for statistics page
</commit_message>
<xml_diff>
--- a/public/excel/branches.xlsx
+++ b/public/excel/branches.xlsx
@@ -36,9 +36,6 @@
     <t>Ташкентский филиал</t>
   </si>
   <si>
-    <t>Сирдарьинский филиал</t>
-  </si>
-  <si>
     <t>Джизакский филиал</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>Каракалпакстанский филиал</t>
+  </si>
+  <si>
+    <t>Сырдарьинский филиал</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,47 +427,47 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
branches.xlsx file spelling fixed
</commit_message>
<xml_diff>
--- a/public/excel/branches.xlsx
+++ b/public/excel/branches.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2562D341-E78E-5D41-9872-EB9ACA6C974A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="22260" windowHeight="12636"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -49,9 +48,6 @@
     <t>Сурхандарьинский филиал</t>
   </si>
   <si>
-    <t>Навоийскиц филиал</t>
-  </si>
-  <si>
     <t>Бухарский филиал</t>
   </si>
   <si>
@@ -62,12 +58,15 @@
   </si>
   <si>
     <t>Сырдарьинский филиал</t>
+  </si>
+  <si>
+    <t>Навоийский филиал</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,7 +110,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,20 +387,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -409,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -417,7 +416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -425,7 +424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -433,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -441,15 +440,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -457,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -465,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -473,7 +472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -481,36 +480,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel import columns
</commit_message>
<xml_diff>
--- a/public/excel/branches.xlsx
+++ b/public/excel/branches.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="22260" windowHeight="12636"/>
+    <workbookView xWindow="0" yWindow="510" windowWidth="22260" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -388,128 +388,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
+      </c>
+      <c r="C14">
+        <v>1735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>